<commit_message>
added jpub books not trelliscopejs
</commit_message>
<xml_diff>
--- a/data/후원도서_한국 R 컨퍼런스.xlsx
+++ b/data/후원도서_한국 R 컨퍼런스.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwangchunlee/swc/ingest-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294F2B5D-BDFD-CD41-B3BA-AF1E81E0562B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F949D26-A76B-3D41-A5C6-2AD795A22951}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="1520" windowWidth="21600" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="한국 R 컨퍼런스20210817" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>제이펍</t>
   </si>
@@ -149,9 +149,6 @@
     <t>키워드</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>판형</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -330,9 +327,6 @@
     <t>25,000원</t>
   </si>
   <si>
-    <t>2021년 2월 11일</t>
-  </si>
-  <si>
     <r>
       <t>979-11-90665-80-3</t>
     </r>
@@ -931,18 +925,6 @@
     <t>48,000원</t>
   </si>
   <si>
-    <t>비모수적 검정</t>
-  </si>
-  <si>
-    <t>다변량분산분석</t>
-  </si>
-  <si>
-    <t>탐색적 인자분석</t>
-  </si>
-  <si>
-    <t>다층 선형모형</t>
-  </si>
-  <si>
     <r>
       <t>Discovering Statistics Using R(</t>
     </r>
@@ -1797,6 +1779,22 @@
       </rPr>
       <t xml:space="preserve"> (93000)</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021년7월20일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019년6월4일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017년12월15일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021년2월11일</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2009,7 +2007,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2042,9 +2040,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2065,6 +2060,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="31" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2384,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2397,12 +2398,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
@@ -2566,7 +2567,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2576,7 +2577,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -2584,40 +2585,40 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="16">
-        <v>44397</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>28</v>
@@ -2625,10 +2626,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2636,23 +2637,23 @@
         <v>30</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16">
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>43</v>
+      <c r="B9" s="16" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2671,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2681,7 +2682,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
@@ -2689,75 +2690,75 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="19" t="s">
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2765,7 +2766,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16">
@@ -2773,15 +2774,15 @@
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2798,7 +2799,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="121.6640625" defaultRowHeight="15"/>
@@ -2808,7 +2809,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -2816,64 +2817,64 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="14" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="16">
+      <c r="A4" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16">
-      <c r="A3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="B4" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
-      <c r="A4" s="21" t="s">
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
-      <c r="A5" s="21" t="s">
-        <v>64</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16">
-        <v>43620</v>
+      <c r="B6" s="25" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>28</v>
@@ -2881,10 +2882,10 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2892,7 +2893,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2900,15 +2901,15 @@
         <v>31</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2925,172 +2926,134 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="138" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="16">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="16">
-      <c r="A2" s="22" t="s">
-        <v>59</v>
+    <row r="2" spans="1:2" ht="16">
+      <c r="A2" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16">
+      <c r="A4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16">
+      <c r="A6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
+      <c r="A7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="16">
-      <c r="A3" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="16">
-      <c r="A4" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="16">
-      <c r="A5" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:2" ht="16">
+      <c r="A8" s="21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="16">
-      <c r="A6" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="16">
-      <c r="A7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="16">
-      <c r="A8" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28">
-      <c r="A10" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="V13" t="s">
-        <v>77</v>
-      </c>
-      <c r="W13" t="s">
-        <v>32</v>
-      </c>
-      <c r="X13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="Y13" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28">
-      <c r="A14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28">
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="10"/>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:2">
       <c r="A16" s="10"/>
     </row>
     <row r="17" spans="1:1">
@@ -3130,7 +3093,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
@@ -3138,72 +3101,72 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16">
-      <c r="A2" s="23" t="s">
-        <v>59</v>
+      <c r="A2" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
-      <c r="A5" s="23" t="s">
-        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16">
-      <c r="A8" s="23" t="s">
-        <v>74</v>
+      <c r="A8" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -3211,7 +3174,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -3222,7 +3185,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="32">
@@ -3230,15 +3193,15 @@
         <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3252,7 +3215,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3262,7 +3225,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -3270,64 +3233,64 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16">
-      <c r="A2" s="24" t="s">
-        <v>59</v>
+      <c r="A2" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
-      <c r="A5" s="24" t="s">
-        <v>64</v>
-      </c>
       <c r="B5" s="14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16">
-        <v>43084</v>
+      <c r="B6" s="26" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>28</v>
@@ -3335,10 +3298,10 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3346,7 +3309,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3354,15 +3317,15 @@
         <v>31</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>